<commit_message>
add timeline as pdf
</commit_message>
<xml_diff>
--- a/Gantt Project Planner.xlsx
+++ b/Gantt Project Planner.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lin\Dropbox\My PC (STU-LOAN-23831)\Desktop\hons final proj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lin\Dropbox\My PC (STU-LOAN-23831)\Desktop\HONSSeniorProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A187157E-ABA1-4A4C-988D-BF1CC988AE4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CC9F01-9412-46FE-BB2F-F1EDA15A5FB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -559,6 +559,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -606,9 +609,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1045,11 +1045,11 @@
       <c r="G1" s="13"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
       <c r="G2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1057,66 +1057,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="33"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="30" t="s">
+      <c r="Q2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="32"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="33"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="22" t="s">
+      <c r="V2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="34"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="35"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="35" t="s">
+      <c r="AA2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="38"/>
       <c r="AH2" s="20"/>
-      <c r="AI2" s="22" t="s">
+      <c r="AI2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="AJ2" s="23"/>
-      <c r="AK2" s="23"/>
-      <c r="AL2" s="23"/>
-      <c r="AM2" s="23"/>
-      <c r="AN2" s="23"/>
-      <c r="AO2" s="23"/>
-      <c r="AP2" s="23"/>
+      <c r="AJ2" s="24"/>
+      <c r="AK2" s="24"/>
+      <c r="AL2" s="24"/>
+      <c r="AM2" s="24"/>
+      <c r="AN2" s="24"/>
+      <c r="AO2" s="24"/>
+      <c r="AP2" s="24"/>
     </row>
     <row r="3" spans="2:67" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="30" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1143,12 +1143,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1347,7 +1347,7 @@
       </c>
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="22" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="7">
@@ -1363,7 +1363,7 @@
       </c>
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="22" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="7">

</xml_diff>